<commit_message>
Changes in figure appearance
Variable labels in the Tables and Figure/Supplements with minor changes
</commit_message>
<xml_diff>
--- a/input data/var_lexicon.xlsx
+++ b/input data/var_lexicon.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="252">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">ref_time</t>
   </si>
   <si>
+    <t xml:space="preserve">label_long</t>
+  </si>
+  <si>
     <t xml:space="preserve">sex</t>
   </si>
   <si>
@@ -193,6 +196,9 @@
     <t xml:space="preserve">reduced DLCO</t>
   </si>
   <si>
+    <t xml:space="preserve">reduced DLCO (&lt; 80%)</t>
+  </si>
+  <si>
     <t xml:space="preserve">lufo_red</t>
   </si>
   <si>
@@ -337,7 +343,7 @@
     <t xml:space="preserve">EF_red</t>
   </si>
   <si>
-    <t xml:space="preserve">reduced EF</t>
+    <t xml:space="preserve">reduced LVEF</t>
   </si>
   <si>
     <t xml:space="preserve">diastolic_dysf</t>
@@ -529,6 +535,9 @@
     <t xml:space="preserve">CT abnormality</t>
   </si>
   <si>
+    <t xml:space="preserve">CT abnormality (CT score ≥ 1)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ct_severity_5</t>
   </si>
   <si>
@@ -583,7 +592,7 @@
     <t xml:space="preserve">smwd_low</t>
   </si>
   <si>
-    <t xml:space="preserve">SMDW &lt; ref.</t>
+    <t xml:space="preserve">SMWD &lt; ref.</t>
   </si>
   <si>
     <t xml:space="preserve">BRCS</t>
@@ -592,6 +601,9 @@
     <t xml:space="preserve">Resilience (BRCS)</t>
   </si>
   <si>
+    <t xml:space="preserve">Resilience score (BRCS)</t>
+  </si>
+  <si>
     <t xml:space="preserve">BRCS_class</t>
   </si>
   <si>
@@ -601,40 +613,58 @@
     <t xml:space="preserve">General health (EQ5D5L VAS)</t>
   </si>
   <si>
+    <t xml:space="preserve">General health score (EQ5D5L VAS)</t>
+  </si>
+  <si>
     <t xml:space="preserve">EQ5DL_mobility</t>
   </si>
   <si>
     <t xml:space="preserve">Mobility impairment (EQ5D5L)</t>
   </si>
   <si>
+    <t xml:space="preserve">Mobility impairment score (EQ5D5L)</t>
+  </si>
+  <si>
     <t xml:space="preserve">EQ5DL_selfcare</t>
   </si>
   <si>
     <t xml:space="preserve">Self-care impairment (EQ5D5L)</t>
   </si>
   <si>
+    <t xml:space="preserve">Self-care impairment score (EQ5D5L)</t>
+  </si>
+  <si>
     <t xml:space="preserve">EQ5DL_activities</t>
   </si>
   <si>
     <t xml:space="preserve">Activity impairment (EQ5D5L)</t>
   </si>
   <si>
+    <t xml:space="preserve">Activity impairment score (EQ5D5L)</t>
+  </si>
+  <si>
     <t xml:space="preserve">EQ5DL_pain</t>
   </si>
   <si>
     <t xml:space="preserve">Pain/discomfort (EQ5D5L)</t>
   </si>
   <si>
+    <t xml:space="preserve">Pain/discomfort score (EQ5D5L)</t>
+  </si>
+  <si>
     <t xml:space="preserve">EQ5DL_anxiety</t>
   </si>
   <si>
     <t xml:space="preserve">Anxiety/depression (EQ5D5L)</t>
   </si>
   <si>
+    <t xml:space="preserve">Anxiety/depression score (EQ5D5L)</t>
+  </si>
+  <si>
     <t xml:space="preserve">EQ5DL_low</t>
   </si>
   <si>
-    <t xml:space="preserve">Imp. general health (EQ5D5L VAS &lt; 73)</t>
+    <t xml:space="preserve">Imp. general health (VAS &lt; 73, EQ5D5L)</t>
   </si>
   <si>
     <t xml:space="preserve">EQ5DL_mobility_bi</t>
@@ -643,36 +673,54 @@
     <t xml:space="preserve">Imp. mobility (EQ5D5L)</t>
   </si>
   <si>
+    <t xml:space="preserve">Imp. mobility (score  &gt; 1, EQ5D5L)</t>
+  </si>
+  <si>
     <t xml:space="preserve">EQ5DL_selfcare_bi</t>
   </si>
   <si>
     <t xml:space="preserve">Imp. self-care (EQ5D5L)</t>
   </si>
   <si>
+    <t xml:space="preserve">Imp. self-care (score  &gt; 1, EQ5D5L)</t>
+  </si>
+  <si>
     <t xml:space="preserve">EQ5DL_activities_bi</t>
   </si>
   <si>
     <t xml:space="preserve">Imp. usual activity (EQ5D5L)</t>
   </si>
   <si>
+    <t xml:space="preserve">Imp. usual activity (score  &gt; 1, EQ5D5L)</t>
+  </si>
+  <si>
     <t xml:space="preserve">EQ5DL_pain_bi</t>
   </si>
   <si>
     <t xml:space="preserve">Pain/discomfort present (EQ5D5L)</t>
   </si>
   <si>
+    <t xml:space="preserve">Pain/discomfort (score  &gt; 1, EQ5D5L)</t>
+  </si>
+  <si>
     <t xml:space="preserve">EQ5DL_anxiety_bi</t>
   </si>
   <si>
     <t xml:space="preserve">Anxiety/depression present (EQ5D5L)</t>
   </si>
   <si>
+    <t xml:space="preserve">Anxiety/depression (score  &gt; 1, EQ5D5L)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chalder_FS</t>
   </si>
   <si>
     <t xml:space="preserve">Fatigue (likert CFS)</t>
   </si>
   <si>
+    <t xml:space="preserve">Fatigue score (likert CFS)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chalder_FS_bimodal</t>
   </si>
   <si>
@@ -685,12 +733,18 @@
     <t xml:space="preserve">Somatic symptom disorder (SSD-12)</t>
   </si>
   <si>
+    <t xml:space="preserve">Somatic symptom disorder score (SSD-12)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stress</t>
   </si>
   <si>
     <t xml:space="preserve">Stress (PSS)</t>
   </si>
   <si>
+    <t xml:space="preserve">Stress score (PSS)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stress_hi</t>
   </si>
   <si>
@@ -703,16 +757,25 @@
     <t xml:space="preserve">Self-efficacy (GSES)</t>
   </si>
   <si>
+    <t xml:space="preserve">Self-efficacy score (GSES)</t>
+  </si>
+  <si>
     <t xml:space="preserve">KW_IPQ</t>
   </si>
   <si>
     <t xml:space="preserve">Illness perception (IPQ)</t>
   </si>
   <si>
+    <t xml:space="preserve">Illness perception score (IPQ)</t>
+  </si>
+  <si>
     <t xml:space="preserve">SOCL9</t>
   </si>
   <si>
     <t xml:space="preserve">Sense of coherence loss (SOCL-9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sense of coherence score (SOCL-9)</t>
   </si>
 </sst>
 </file>
@@ -813,17 +876,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F115"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B109" activeCellId="0" sqref="B109"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G88" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G94" activeCellId="0" sqref="G94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,1988 +909,2321 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>9</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="G3" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="E5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="G9" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="G11" s="0" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="G12" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>32</v>
-      </c>
       <c r="C14" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="C16" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="C21" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F54" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="G54" s="0" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F55" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="G55" s="0" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F56" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="G56" s="0" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F57" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G57" s="0" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F58" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G58" s="0" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F59" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G59" s="0" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F60" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G60" s="0" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F61" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G61" s="0" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F62" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G62" s="0" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F63" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G63" s="0" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F64" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G64" s="0" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F65" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G65" s="0" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F66" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G66" s="0" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F67" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G67" s="0" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F68" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G68" s="0" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F69" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G69" s="0" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G70" s="0" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G74" s="0" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G76" s="0" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G79" s="0" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G80" s="0" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+      <c r="G83" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F86" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G86" s="0" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F87" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G87" s="0" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B88" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="F88" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G88" s="0" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F89" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G89" s="0" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F90" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G90" s="0" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F91" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G91" s="0" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C92" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="B92" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>181</v>
-      </c>
       <c r="D92" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F92" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G92" s="0" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F93" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G93" s="0" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F94" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G94" s="0" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F95" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G95" s="0" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F96" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G96" s="0" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F97" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G97" s="0" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F98" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G98" s="0" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F99" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G99" s="0" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F100" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G100" s="0" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F101" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G101" s="0" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F102" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G102" s="0" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F103" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G103" s="0" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F104" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G104" s="0" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F105" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G105" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F106" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G106" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F107" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G107" s="0" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F108" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="109" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G108" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F109" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G109" s="0" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F110" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G110" s="0" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F111" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G111" s="0" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F112" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G112" s="0" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>225</v>
+        <v>243</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>226</v>
+        <v>244</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F113" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G113" s="0" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>228</v>
+        <v>247</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F114" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G114" s="0" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F115" s="0" t="n">
         <v>4</v>
+      </c>
+      <c r="G115" s="0" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Analysis and manuscript revision
Changes of the pipeline requested by the reviewers. Improved clarity of Supplementary Material
</commit_message>
<xml_diff>
--- a/input data/var_lexicon.xlsx
+++ b/input data/var_lexicon.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="268">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -169,31 +169,43 @@
     <t xml:space="preserve">FVC_red</t>
   </si>
   <si>
-    <t xml:space="preserve">reduced FVC</t>
+    <t xml:space="preserve">FVC &lt; 80%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reduced FVC (&lt; 80%)</t>
   </si>
   <si>
     <t xml:space="preserve">FEV1_red</t>
   </si>
   <si>
-    <t xml:space="preserve">reduced FEV1</t>
+    <t xml:space="preserve">FEV1 &lt; 80%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reduced FEV1 (&lt; 80%)</t>
   </si>
   <si>
     <t xml:space="preserve">FEV1_FVC_red</t>
   </si>
   <si>
-    <t xml:space="preserve">reduced FEV1:FVC</t>
+    <t xml:space="preserve">FEV1:FVC &lt; 70%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reduced FEV1:FVC (&lt; 70%)</t>
   </si>
   <si>
     <t xml:space="preserve">TLC_red</t>
   </si>
   <si>
-    <t xml:space="preserve">reduced TLC</t>
+    <t xml:space="preserve">TLC &lt; 80%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reduced TLC (&lt; 80%)</t>
   </si>
   <si>
     <t xml:space="preserve">DLCO_red</t>
   </si>
   <si>
-    <t xml:space="preserve">reduced DLCO</t>
+    <t xml:space="preserve">DLCO &lt; 80%</t>
   </si>
   <si>
     <t xml:space="preserve">reduced DLCO (&lt; 80%)</t>
@@ -289,7 +301,7 @@
     <t xml:space="preserve">NtproBNP_elv</t>
   </si>
   <si>
-    <t xml:space="preserve">elevated NT-proBNP</t>
+    <t xml:space="preserve">NT-proBNP &gt;150 pg/mL</t>
   </si>
   <si>
     <t xml:space="preserve">DDimer</t>
@@ -301,7 +313,7 @@
     <t xml:space="preserve">Ddimer_elv</t>
   </si>
   <si>
-    <t xml:space="preserve">elevated D-dimer</t>
+    <t xml:space="preserve">D-dimer &gt;500 µg/L</t>
   </si>
   <si>
     <t xml:space="preserve">CRP</t>
@@ -310,7 +322,7 @@
     <t xml:space="preserve">CRP_elv</t>
   </si>
   <si>
-    <t xml:space="preserve">elevated CRP</t>
+    <t xml:space="preserve">CRP &gt;0.5 mg/L</t>
   </si>
   <si>
     <t xml:space="preserve">PCT</t>
@@ -319,7 +331,7 @@
     <t xml:space="preserve">PCT_elv</t>
   </si>
   <si>
-    <t xml:space="preserve">elevated PCT</t>
+    <t xml:space="preserve">PCT &gt;0.15 µg/L</t>
   </si>
   <si>
     <t xml:space="preserve">IL6</t>
@@ -328,7 +340,7 @@
     <t xml:space="preserve">IL6_elv</t>
   </si>
   <si>
-    <t xml:space="preserve">elevated IL6</t>
+    <t xml:space="preserve">IL6 &gt;7 pg/mL</t>
   </si>
   <si>
     <t xml:space="preserve">HbA1c</t>
@@ -337,7 +349,7 @@
     <t xml:space="preserve">HbA1c_elv</t>
   </si>
   <si>
-    <t xml:space="preserve">elevated HbA1c</t>
+    <t xml:space="preserve">HbA1c &gt;5.6%</t>
   </si>
   <si>
     <t xml:space="preserve">EF_red</t>
@@ -358,6 +370,9 @@
     <t xml:space="preserve"># comorbidities</t>
   </si>
   <si>
+    <t xml:space="preserve">Number of comorbidities</t>
+  </si>
+  <si>
     <t xml:space="preserve">comorb_present</t>
   </si>
   <si>
@@ -370,6 +385,9 @@
     <t xml:space="preserve">CVD</t>
   </si>
   <si>
+    <t xml:space="preserve">Cardiovascular disease</t>
+  </si>
+  <si>
     <t xml:space="preserve">hypertension_comorb</t>
   </si>
   <si>
@@ -424,12 +442,18 @@
     <t xml:space="preserve">CKD</t>
   </si>
   <si>
+    <t xml:space="preserve">Chronic kidney disease</t>
+  </si>
+  <si>
     <t xml:space="preserve">gastro_comorb</t>
   </si>
   <si>
     <t xml:space="preserve">GID</t>
   </si>
   <si>
+    <t xml:space="preserve">Gastrointestinal disease</t>
+  </si>
+  <si>
     <t xml:space="preserve">cldis_comorb</t>
   </si>
   <si>
@@ -448,15 +472,54 @@
     <t xml:space="preserve">Immune deficiency</t>
   </si>
   <si>
+    <t xml:space="preserve">treat_steroids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steroid therapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treat_antiinfec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti-infective therapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treat_macrolides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrolide therapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treat_antiplat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti-platelet therapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treat_anticoag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti-coagulation therapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treat_immunosuppr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Immunosuppression</t>
+  </si>
+  <si>
     <t xml:space="preserve">mmrc</t>
   </si>
   <si>
-    <t xml:space="preserve">mMRC</t>
+    <t xml:space="preserve">Dyspnea score (mMRC)</t>
   </si>
   <si>
     <t xml:space="preserve">ECOG</t>
   </si>
   <si>
+    <t xml:space="preserve">Physical performance score (ECOG)</t>
+  </si>
+  <si>
     <t xml:space="preserve">sympt_present</t>
   </si>
   <si>
@@ -469,6 +532,9 @@
     <t xml:space="preserve"># symptoms</t>
   </si>
   <si>
+    <t xml:space="preserve">Number of symptoms</t>
+  </si>
+  <si>
     <t xml:space="preserve">sleep_sympt</t>
   </si>
   <si>
@@ -478,7 +544,7 @@
     <t xml:space="preserve">dyspnoe_sympt</t>
   </si>
   <si>
-    <t xml:space="preserve">Dyspnea</t>
+    <t xml:space="preserve">Dyspnea (mMRC ≥1)</t>
   </si>
   <si>
     <t xml:space="preserve">cough_sympt</t>
@@ -496,13 +562,13 @@
     <t xml:space="preserve">night_sweat_sympt</t>
   </si>
   <si>
-    <t xml:space="preserve">Night sweat</t>
+    <t xml:space="preserve">Night sweating</t>
   </si>
   <si>
     <t xml:space="preserve">gastro_sympt</t>
   </si>
   <si>
-    <t xml:space="preserve">Gastrointestinal</t>
+    <t xml:space="preserve">Gastrointestinal symptoms</t>
   </si>
   <si>
     <t xml:space="preserve">anosmia_sympt</t>
@@ -514,7 +580,7 @@
     <t xml:space="preserve">fatigue_sympt</t>
   </si>
   <si>
-    <t xml:space="preserve">Reduced performance</t>
+    <t xml:space="preserve">Reduced performance (ECOG ≥1) </t>
   </si>
   <si>
     <t xml:space="preserve">pain_sympt</t>
@@ -532,16 +598,13 @@
     <t xml:space="preserve">ct_severity_any</t>
   </si>
   <si>
-    <t xml:space="preserve">CT abnormality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CT abnormality (CT score ≥ 1)</t>
+    <t xml:space="preserve">CT abnormality (CT score ≥1)</t>
   </si>
   <si>
     <t xml:space="preserve">ct_severity_5</t>
   </si>
   <si>
-    <t xml:space="preserve">CT severity score &gt; 5</t>
+    <t xml:space="preserve">CT severity score &gt;5</t>
   </si>
   <si>
     <t xml:space="preserve">SarsCov2_IgG</t>
@@ -565,13 +628,13 @@
     <t xml:space="preserve">derma_sympt</t>
   </si>
   <si>
-    <t xml:space="preserve">Dermatological</t>
+    <t xml:space="preserve">Dermatological symptoms</t>
   </si>
   <si>
     <t xml:space="preserve">smwd</t>
   </si>
   <si>
-    <t xml:space="preserve">SMWD</t>
+    <t xml:space="preserve">6MWD</t>
   </si>
   <si>
     <t xml:space="preserve">m</t>
@@ -580,19 +643,19 @@
     <t xml:space="preserve">smwd_dref</t>
   </si>
   <si>
-    <t xml:space="preserve">SMWD vs ref.</t>
+    <t xml:space="preserve">6MWD vs ref.</t>
   </si>
   <si>
     <t xml:space="preserve">smwd_dlower</t>
   </si>
   <si>
-    <t xml:space="preserve">SMWD vs LLN</t>
+    <t xml:space="preserve">6MWD vs LLN</t>
   </si>
   <si>
     <t xml:space="preserve">smwd_low</t>
   </si>
   <si>
-    <t xml:space="preserve">SMWD &lt; ref.</t>
+    <t xml:space="preserve">6MWD &lt; ref.</t>
   </si>
   <si>
     <t xml:space="preserve">BRCS</t>
@@ -664,52 +727,37 @@
     <t xml:space="preserve">EQ5DL_low</t>
   </si>
   <si>
-    <t xml:space="preserve">Imp. general health (VAS &lt; 73, EQ5D5L)</t>
+    <t xml:space="preserve">Imp. general health (VAS &lt;73, EQ5D5L)</t>
   </si>
   <si>
     <t xml:space="preserve">EQ5DL_mobility_bi</t>
   </si>
   <si>
-    <t xml:space="preserve">Imp. mobility (EQ5D5L)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imp. mobility (score  &gt; 1, EQ5D5L)</t>
+    <t xml:space="preserve">Imp. mobility (score &gt;1, EQ5D5L)</t>
   </si>
   <si>
     <t xml:space="preserve">EQ5DL_selfcare_bi</t>
   </si>
   <si>
-    <t xml:space="preserve">Imp. self-care (EQ5D5L)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imp. self-care (score  &gt; 1, EQ5D5L)</t>
+    <t xml:space="preserve">Imp. self-care (score &gt;1, EQ5D5L)</t>
   </si>
   <si>
     <t xml:space="preserve">EQ5DL_activities_bi</t>
   </si>
   <si>
-    <t xml:space="preserve">Imp. usual activity (EQ5D5L)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imp. usual activity (score  &gt; 1, EQ5D5L)</t>
+    <t xml:space="preserve">Imp. usual activity (score &gt;1, EQ5D5L)</t>
   </si>
   <si>
     <t xml:space="preserve">EQ5DL_pain_bi</t>
   </si>
   <si>
-    <t xml:space="preserve">Pain/discomfort present (EQ5D5L)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pain/discomfort (score  &gt; 1, EQ5D5L)</t>
+    <t xml:space="preserve">Pain/discomfort (score &gt;1, EQ5D5L)</t>
   </si>
   <si>
     <t xml:space="preserve">EQ5DL_anxiety_bi</t>
   </si>
   <si>
-    <t xml:space="preserve">Anxiety/depression present (EQ5D5L)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anxiety/depression (score  &gt; 1, EQ5D5L)</t>
+    <t xml:space="preserve">Anxiety/depression (score &gt;1, EQ5D5L)</t>
   </si>
   <si>
     <t xml:space="preserve">Chalder_FS</t>
@@ -724,7 +772,7 @@
     <t xml:space="preserve">Chalder_FS_bimodal</t>
   </si>
   <si>
-    <t xml:space="preserve">Fatigue (bimodal CFS ≥ 4)</t>
+    <t xml:space="preserve">Fatigue (bimodal CFS ≥4)</t>
   </si>
   <si>
     <t xml:space="preserve">SSD12</t>
@@ -748,7 +796,7 @@
     <t xml:space="preserve">Stress_hi</t>
   </si>
   <si>
-    <t xml:space="preserve">Elevated stress (PSS &gt; 5)</t>
+    <t xml:space="preserve">Elevated stress (PSS &gt;5)</t>
   </si>
   <si>
     <t xml:space="preserve">SES</t>
@@ -876,13 +924,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G115"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G88" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G94" activeCellId="0" sqref="G94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B67" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G79" activeCellId="0" sqref="G79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.17"/>
@@ -1288,15 +1336,15 @@
         <v>35</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>27</v>
@@ -1308,15 +1356,15 @@
         <v>35</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>27</v>
@@ -1328,15 +1376,15 @@
         <v>35</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>27</v>
@@ -1348,15 +1396,15 @@
         <v>35</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>27</v>
@@ -1368,15 +1416,15 @@
         <v>35</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>27</v>
@@ -1388,15 +1436,15 @@
         <v>35</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>14</v>
@@ -1405,15 +1453,15 @@
         <v>16</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>27</v>
@@ -1425,15 +1473,15 @@
         <v>16</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>27</v>
@@ -1445,15 +1493,15 @@
         <v>16</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>27</v>
@@ -1465,18 +1513,18 @@
         <v>16</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>14</v>
@@ -1485,15 +1533,15 @@
         <v>35</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>27</v>
@@ -1505,18 +1553,18 @@
         <v>35</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>14</v>
@@ -1525,15 +1573,15 @@
         <v>35</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>27</v>
@@ -1545,15 +1593,15 @@
         <v>35</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>27</v>
@@ -1565,15 +1613,15 @@
         <v>35</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>27</v>
@@ -1585,18 +1633,18 @@
         <v>35</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>14</v>
@@ -1605,18 +1653,18 @@
         <v>35</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>14</v>
@@ -1625,18 +1673,18 @@
         <v>35</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>14</v>
@@ -1645,15 +1693,15 @@
         <v>35</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>27</v>
@@ -1665,18 +1713,18 @@
         <v>35</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>14</v>
@@ -1685,15 +1733,15 @@
         <v>35</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>27</v>
@@ -1705,18 +1753,18 @@
         <v>35</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>14</v>
@@ -1725,15 +1773,15 @@
         <v>35</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>27</v>
@@ -1745,18 +1793,18 @@
         <v>35</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>14</v>
@@ -1765,15 +1813,15 @@
         <v>35</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>27</v>
@@ -1785,18 +1833,18 @@
         <v>35</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>14</v>
@@ -1805,15 +1853,15 @@
         <v>35</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>27</v>
@@ -1825,15 +1873,15 @@
         <v>35</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>27</v>
@@ -1845,15 +1893,15 @@
         <v>35</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>27</v>
@@ -1865,15 +1913,15 @@
         <v>35</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>27</v>
@@ -1885,15 +1933,15 @@
         <v>35</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>27</v>
@@ -1905,15 +1953,15 @@
         <v>35</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>14</v>
@@ -1925,15 +1973,15 @@
         <v>0</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>27</v>
@@ -1948,15 +1996,15 @@
         <v>0</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>27</v>
@@ -1971,15 +2019,15 @@
         <v>0</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>27</v>
@@ -1994,15 +2042,15 @@
         <v>0</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>27</v>
@@ -2017,15 +2065,15 @@
         <v>0</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>27</v>
@@ -2040,15 +2088,15 @@
         <v>0</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>27</v>
@@ -2063,15 +2111,15 @@
         <v>0</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>27</v>
@@ -2086,15 +2134,15 @@
         <v>0</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>27</v>
@@ -2109,15 +2157,15 @@
         <v>0</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>27</v>
@@ -2132,15 +2180,15 @@
         <v>0</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>27</v>
@@ -2155,15 +2203,15 @@
         <v>0</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>27</v>
@@ -2178,15 +2226,15 @@
         <v>0</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>27</v>
@@ -2201,15 +2249,15 @@
         <v>0</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C67" s="0" t="s">
         <v>27</v>
@@ -2224,15 +2272,15 @@
         <v>0</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>27</v>
@@ -2247,15 +2295,15 @@
         <v>0</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>27</v>
@@ -2270,49 +2318,61 @@
         <v>0</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>35</v>
+        <v>151</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>35</v>
+        <v>10</v>
+      </c>
+      <c r="F71" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>27</v>
@@ -2321,35 +2381,44 @@
         <v>9</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>35</v>
+        <v>10</v>
+      </c>
+      <c r="F72" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
-        <v>147</v>
+      <c r="A73" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>148</v>
+        <v>157</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>35</v>
+        <v>10</v>
+      </c>
+      <c r="F73" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>27</v>
@@ -2358,18 +2427,21 @@
         <v>9</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>35</v>
+        <v>10</v>
+      </c>
+      <c r="F74" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>27</v>
@@ -2378,58 +2450,55 @@
         <v>9</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>35</v>
+        <v>10</v>
+      </c>
+      <c r="F75" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E76" s="0" t="s">
         <v>35</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>27</v>
+        <v>165</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C78" s="0" t="s">
         <v>27</v>
@@ -2441,35 +2510,32 @@
         <v>35</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>27</v>
+        <v>169</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="C80" s="0" t="s">
         <v>27</v>
@@ -2481,15 +2547,15 @@
         <v>35</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="C81" s="0" t="s">
         <v>27</v>
@@ -2501,15 +2567,15 @@
         <v>35</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C82" s="0" t="s">
         <v>27</v>
@@ -2521,32 +2587,35 @@
         <v>35</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>168</v>
+        <v>178</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="C84" s="0" t="s">
         <v>27</v>
@@ -2558,15 +2627,15 @@
         <v>35</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="C85" s="0" t="s">
         <v>27</v>
@@ -2578,55 +2647,55 @@
         <v>35</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="D86" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E86" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="F86" s="0" t="n">
-        <v>1</v>
+        <v>184</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="D87" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E87" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="F87" s="0" t="n">
-        <v>1</v>
+        <v>186</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>27</v>
@@ -2635,457 +2704,439 @@
         <v>9</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F88" s="0" t="n">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="C89" s="0" t="s">
-        <v>27</v>
+        <v>190</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F89" s="0" t="n">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="D90" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E90" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="F90" s="0" t="n">
-        <v>4</v>
+        <v>27</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="D91" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E91" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="F91" s="0" t="n">
-        <v>4</v>
+        <v>27</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="D92" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>16</v>
+        <v>197</v>
       </c>
       <c r="F92" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="C93" s="0" t="s">
-        <v>27</v>
+        <v>196</v>
       </c>
       <c r="D93" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F93" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>192</v>
+        <v>200</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F94" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="D95" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E95" s="0" t="s">
-        <v>176</v>
+        <v>202</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="F95" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G95" s="0" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>176</v>
+        <v>205</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E96" s="0" t="s">
+        <v>197</v>
       </c>
       <c r="F96" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>176</v>
+        <v>207</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E97" s="0" t="s">
+        <v>197</v>
       </c>
       <c r="F97" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>176</v>
+        <v>209</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E98" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="F98" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>176</v>
+        <v>211</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" s="0" t="s">
+        <v>197</v>
       </c>
       <c r="F99" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F100" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>176</v>
+        <v>213</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" s="0" t="s">
+        <v>197</v>
       </c>
       <c r="F101" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C102" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F102" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G102" s="0" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="C103" s="0" t="s">
-        <v>27</v>
+        <v>220</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F103" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="C104" s="0" t="s">
-        <v>27</v>
+        <v>223</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F104" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G104" s="0" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="C105" s="0" t="s">
-        <v>27</v>
+        <v>226</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F105" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G105" s="0" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="C106" s="0" t="s">
-        <v>27</v>
+        <v>229</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F106" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G106" s="0" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="C107" s="0" t="s">
-        <v>27</v>
+        <v>232</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F107" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G107" s="0" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F108" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G108" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C109" s="0" t="s">
         <v>27</v>
@@ -3094,61 +3145,67 @@
         <v>9</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F109" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F110" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G110" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F111" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G111" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C112" s="0" t="s">
         <v>27</v>
@@ -3157,27 +3214,30 @@
         <v>9</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F112" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G112" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F113" s="0" t="n">
         <v>4</v>
@@ -3197,7 +3257,7 @@
         <v>14</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F114" s="0" t="n">
         <v>4</v>
@@ -3213,17 +3273,143 @@
       <c r="B115" s="0" t="s">
         <v>250</v>
       </c>
+      <c r="C115" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="D115" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F115" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G115" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
         <v>251</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F116" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G116" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F117" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G117" s="0" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F118" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G118" s="0" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F119" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G119" s="0" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F120" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G120" s="0" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F121" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G121" s="0" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>